<commit_message>
update constraint on GLD to 1% in sectors_constrained
</commit_message>
<xml_diff>
--- a/data/2_basic_asset_classes_plus_sectors_constrained.xlsx
+++ b/data/2_basic_asset_classes_plus_sectors_constrained.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{AB83254D-652A-415C-924D-81A9C09D9798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DCF545F-470D-4528-9A9B-5C41804F658F}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{AB83254D-652A-415C-924D-81A9C09D9798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D2E91B4-0DC6-4A5E-8E30-0D7F0BB4E265}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -171,13 +171,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -195,6 +195,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,7 +492,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="7">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add OILK to sectors
</commit_message>
<xml_diff>
--- a/data/2_basic_asset_classes_plus_sectors_constrained.xlsx
+++ b/data/2_basic_asset_classes_plus_sectors_constrained.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{AB83254D-652A-415C-924D-81A9C09D9798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D2E91B4-0DC6-4A5E-8E30-0D7F0BB4E265}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{AB83254D-652A-415C-924D-81A9C09D9798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{642524EC-CBE0-4305-B490-A28FF28760B6}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Ticker</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>XLU</t>
+  </si>
+  <si>
+    <t>OILK</t>
   </si>
 </sst>
 </file>
@@ -195,10 +198,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,7 +488,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -705,13 +704,24 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="7">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B20" s="7">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated constraints on sectors to 10%
</commit_message>
<xml_diff>
--- a/data/2_basic_asset_classes_plus_sectors_constrained.xlsx
+++ b/data/2_basic_asset_classes_plus_sectors_constrained.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{AB83254D-652A-415C-924D-81A9C09D9798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{642524EC-CBE0-4305-B490-A28FF28760B6}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{AB83254D-652A-415C-924D-81A9C09D9798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A7D651E-373A-4C1B-867F-1A98BE767985}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,6 +198,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,7 +495,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -568,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -579,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -590,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -601,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -612,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -623,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -634,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -645,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -656,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -667,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>